<commit_message>
code uploaded for BookSwagonStore
</commit_message>
<xml_diff>
--- a/ExcelData/loginSheet.xlsx
+++ b/ExcelData/loginSheet.xlsx
@@ -18,22 +18,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>result</t>
-  </si>
-  <si>
     <t>meghnaborkar23@gmail.com</t>
   </si>
   <si>
     <t>Valid</t>
   </si>
   <si>
-    <t xml:space="preserve"> password</t>
-  </si>
-  <si>
     <t>InValid</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,47 +397,50 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>158921359</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>158921359</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4">
         <v>9158921359</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>